<commit_message>
Final updates, mostly a tidyup for the code, and updated for the 23rd (and likely final) round
</commit_message>
<xml_diff>
--- a/afl-2024-UTC.xlsx
+++ b/afl-2024-UTC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\ML1PEPF00010B20\EXCELCNV\aae69829-9339-459a-926b-6d207d618135\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{004DDE84-9079-471F-850E-B4A455F14C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1242" documentId="8_{3316E54F-DE3D-49FF-A317-FCBAD4945F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{282AC71D-AAD9-4F10-BB44-E564123FC329}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{8B794961-40E5-41C4-9314-4DD18F7FF2BC}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="374">
   <si>
     <t>Match Number</t>
   </si>
@@ -1110,25 +1110,79 @@
     <t>39 - 124</t>
   </si>
   <si>
+    <t>89 - 86</t>
+  </si>
+  <si>
+    <t>64 - 82</t>
+  </si>
+  <si>
+    <t>97 - 102</t>
+  </si>
+  <si>
+    <t>62 - 73</t>
+  </si>
+  <si>
+    <t>86 - 87</t>
+  </si>
+  <si>
+    <t>51 - 53</t>
+  </si>
+  <si>
+    <t>38 - 112</t>
+  </si>
+  <si>
+    <t>51 - 99</t>
+  </si>
+  <si>
+    <t>111 - 72</t>
+  </si>
+  <si>
     <t>16/08/2024 09:40</t>
   </si>
   <si>
+    <t>59 - 98</t>
+  </si>
+  <si>
     <t>17/08/2024 03:45</t>
   </si>
   <si>
+    <t>63 - 117</t>
+  </si>
+  <si>
+    <t>101 - 92</t>
+  </si>
+  <si>
     <t>17/08/2024 06:35</t>
   </si>
   <si>
+    <t>79 - 78</t>
+  </si>
+  <si>
     <t>17/08/2024 09:30</t>
   </si>
   <si>
+    <t>107 - 89</t>
+  </si>
+  <si>
+    <t>80 - 58</t>
+  </si>
+  <si>
     <t>18/08/2024 03:10</t>
   </si>
   <si>
+    <t>138 - 42</t>
+  </si>
+  <si>
     <t>18/08/2024 05:20</t>
   </si>
   <si>
+    <t>131 - 68</t>
+  </si>
+  <si>
     <t>18/08/2024 06:40</t>
+  </si>
+  <si>
+    <t>34 - 99</t>
   </si>
   <si>
     <t>23/08/2024 02:00</t>
@@ -2008,8 +2062,8 @@
   <dimension ref="A1:AE208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="J168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE182" sqref="AE182"/>
+      <pane ySplit="1" topLeftCell="B171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE200" sqref="AE200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2029,7 +2083,7 @@
     <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" customWidth="1"/>
     <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -19251,6 +19305,81 @@
       <c r="F182" t="s">
         <v>46</v>
       </c>
+      <c r="G182" t="s">
+        <v>347</v>
+      </c>
+      <c r="H182">
+        <v>1</v>
+      </c>
+      <c r="I182">
+        <v>1</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+      <c r="K182">
+        <v>1</v>
+      </c>
+      <c r="L182">
+        <v>1</v>
+      </c>
+      <c r="M182">
+        <v>1</v>
+      </c>
+      <c r="N182">
+        <v>1</v>
+      </c>
+      <c r="O182">
+        <v>1</v>
+      </c>
+      <c r="P182">
+        <v>1</v>
+      </c>
+      <c r="Q182">
+        <v>1</v>
+      </c>
+      <c r="R182">
+        <v>1</v>
+      </c>
+      <c r="S182">
+        <v>0</v>
+      </c>
+      <c r="T182">
+        <v>1</v>
+      </c>
+      <c r="U182">
+        <v>0</v>
+      </c>
+      <c r="V182">
+        <v>1</v>
+      </c>
+      <c r="W182">
+        <v>1</v>
+      </c>
+      <c r="X182">
+        <v>1</v>
+      </c>
+      <c r="Y182">
+        <v>1</v>
+      </c>
+      <c r="Z182">
+        <v>-1</v>
+      </c>
+      <c r="AA182">
+        <v>1</v>
+      </c>
+      <c r="AB182">
+        <v>1</v>
+      </c>
+      <c r="AC182">
+        <v>1</v>
+      </c>
+      <c r="AD182">
+        <v>1</v>
+      </c>
+      <c r="AE182">
+        <v>1</v>
+      </c>
     </row>
     <row r="183" spans="1:31">
       <c r="A183">
@@ -19271,6 +19400,81 @@
       <c r="F183" t="s">
         <v>45</v>
       </c>
+      <c r="G183" t="s">
+        <v>348</v>
+      </c>
+      <c r="H183">
+        <v>1</v>
+      </c>
+      <c r="I183">
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+      <c r="K183">
+        <v>1</v>
+      </c>
+      <c r="L183">
+        <v>1</v>
+      </c>
+      <c r="M183">
+        <v>1</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="O183">
+        <v>1</v>
+      </c>
+      <c r="P183">
+        <v>1</v>
+      </c>
+      <c r="Q183">
+        <v>1</v>
+      </c>
+      <c r="R183">
+        <v>1</v>
+      </c>
+      <c r="S183">
+        <v>1</v>
+      </c>
+      <c r="T183">
+        <v>1</v>
+      </c>
+      <c r="U183">
+        <v>1</v>
+      </c>
+      <c r="V183">
+        <v>1</v>
+      </c>
+      <c r="W183">
+        <v>1</v>
+      </c>
+      <c r="X183">
+        <v>1</v>
+      </c>
+      <c r="Y183">
+        <v>1</v>
+      </c>
+      <c r="Z183">
+        <v>-1</v>
+      </c>
+      <c r="AA183">
+        <v>1</v>
+      </c>
+      <c r="AB183">
+        <v>1</v>
+      </c>
+      <c r="AC183">
+        <v>1</v>
+      </c>
+      <c r="AD183">
+        <v>1</v>
+      </c>
+      <c r="AE183">
+        <v>1</v>
+      </c>
     </row>
     <row r="184" spans="1:31">
       <c r="A184">
@@ -19291,6 +19495,81 @@
       <c r="F184" t="s">
         <v>74</v>
       </c>
+      <c r="G184" t="s">
+        <v>349</v>
+      </c>
+      <c r="H184">
+        <v>1</v>
+      </c>
+      <c r="I184">
+        <v>1</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>1</v>
+      </c>
+      <c r="L184">
+        <v>1</v>
+      </c>
+      <c r="M184">
+        <v>1</v>
+      </c>
+      <c r="N184">
+        <v>1</v>
+      </c>
+      <c r="O184">
+        <v>1</v>
+      </c>
+      <c r="P184">
+        <v>1</v>
+      </c>
+      <c r="Q184">
+        <v>1</v>
+      </c>
+      <c r="R184">
+        <v>1</v>
+      </c>
+      <c r="S184">
+        <v>0</v>
+      </c>
+      <c r="T184">
+        <v>0</v>
+      </c>
+      <c r="U184">
+        <v>1</v>
+      </c>
+      <c r="V184">
+        <v>1</v>
+      </c>
+      <c r="W184">
+        <v>1</v>
+      </c>
+      <c r="X184">
+        <v>1</v>
+      </c>
+      <c r="Y184">
+        <v>1</v>
+      </c>
+      <c r="Z184">
+        <v>-1</v>
+      </c>
+      <c r="AA184">
+        <v>1</v>
+      </c>
+      <c r="AB184">
+        <v>1</v>
+      </c>
+      <c r="AC184">
+        <v>1</v>
+      </c>
+      <c r="AD184">
+        <v>1</v>
+      </c>
+      <c r="AE184">
+        <v>1</v>
+      </c>
     </row>
     <row r="185" spans="1:31">
       <c r="A185">
@@ -19311,6 +19590,81 @@
       <c r="F185" t="s">
         <v>62</v>
       </c>
+      <c r="G185" t="s">
+        <v>350</v>
+      </c>
+      <c r="H185">
+        <v>1</v>
+      </c>
+      <c r="I185">
+        <v>1</v>
+      </c>
+      <c r="J185">
+        <v>1</v>
+      </c>
+      <c r="K185">
+        <v>1</v>
+      </c>
+      <c r="L185">
+        <v>1</v>
+      </c>
+      <c r="M185">
+        <v>1</v>
+      </c>
+      <c r="N185">
+        <v>1</v>
+      </c>
+      <c r="O185">
+        <v>1</v>
+      </c>
+      <c r="P185">
+        <v>1</v>
+      </c>
+      <c r="Q185">
+        <v>1</v>
+      </c>
+      <c r="R185">
+        <v>1</v>
+      </c>
+      <c r="S185">
+        <v>1</v>
+      </c>
+      <c r="T185">
+        <v>0</v>
+      </c>
+      <c r="U185">
+        <v>0</v>
+      </c>
+      <c r="V185">
+        <v>0</v>
+      </c>
+      <c r="W185">
+        <v>1</v>
+      </c>
+      <c r="X185">
+        <v>1</v>
+      </c>
+      <c r="Y185">
+        <v>1</v>
+      </c>
+      <c r="Z185">
+        <v>-1</v>
+      </c>
+      <c r="AA185">
+        <v>1</v>
+      </c>
+      <c r="AB185">
+        <v>1</v>
+      </c>
+      <c r="AC185">
+        <v>1</v>
+      </c>
+      <c r="AD185">
+        <v>1</v>
+      </c>
+      <c r="AE185">
+        <v>1</v>
+      </c>
     </row>
     <row r="186" spans="1:31">
       <c r="A186">
@@ -19331,6 +19685,81 @@
       <c r="F186" t="s">
         <v>41</v>
       </c>
+      <c r="G186" t="s">
+        <v>351</v>
+      </c>
+      <c r="H186">
+        <v>1</v>
+      </c>
+      <c r="I186">
+        <v>1</v>
+      </c>
+      <c r="J186">
+        <v>1</v>
+      </c>
+      <c r="K186">
+        <v>1</v>
+      </c>
+      <c r="L186">
+        <v>1</v>
+      </c>
+      <c r="M186">
+        <v>1</v>
+      </c>
+      <c r="N186">
+        <v>1</v>
+      </c>
+      <c r="O186">
+        <v>1</v>
+      </c>
+      <c r="P186">
+        <v>1</v>
+      </c>
+      <c r="Q186">
+        <v>1</v>
+      </c>
+      <c r="R186">
+        <v>1</v>
+      </c>
+      <c r="S186">
+        <v>1</v>
+      </c>
+      <c r="T186">
+        <v>0</v>
+      </c>
+      <c r="U186">
+        <v>1</v>
+      </c>
+      <c r="V186">
+        <v>1</v>
+      </c>
+      <c r="W186">
+        <v>1</v>
+      </c>
+      <c r="X186">
+        <v>1</v>
+      </c>
+      <c r="Y186">
+        <v>1</v>
+      </c>
+      <c r="Z186">
+        <v>-1</v>
+      </c>
+      <c r="AA186">
+        <v>1</v>
+      </c>
+      <c r="AB186">
+        <v>1</v>
+      </c>
+      <c r="AC186">
+        <v>1</v>
+      </c>
+      <c r="AD186">
+        <v>1</v>
+      </c>
+      <c r="AE186">
+        <v>1</v>
+      </c>
     </row>
     <row r="187" spans="1:31">
       <c r="A187">
@@ -19351,6 +19780,81 @@
       <c r="F187" t="s">
         <v>73</v>
       </c>
+      <c r="G187" t="s">
+        <v>352</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+      <c r="K187">
+        <v>0</v>
+      </c>
+      <c r="L187">
+        <v>0</v>
+      </c>
+      <c r="M187">
+        <v>0</v>
+      </c>
+      <c r="N187">
+        <v>0</v>
+      </c>
+      <c r="O187">
+        <v>0</v>
+      </c>
+      <c r="P187">
+        <v>0</v>
+      </c>
+      <c r="Q187">
+        <v>0</v>
+      </c>
+      <c r="R187">
+        <v>0</v>
+      </c>
+      <c r="S187">
+        <v>0</v>
+      </c>
+      <c r="T187">
+        <v>0</v>
+      </c>
+      <c r="U187">
+        <v>0</v>
+      </c>
+      <c r="V187">
+        <v>0</v>
+      </c>
+      <c r="W187">
+        <v>0</v>
+      </c>
+      <c r="X187">
+        <v>0</v>
+      </c>
+      <c r="Y187">
+        <v>0</v>
+      </c>
+      <c r="Z187">
+        <v>-1</v>
+      </c>
+      <c r="AA187">
+        <v>0</v>
+      </c>
+      <c r="AB187">
+        <v>0</v>
+      </c>
+      <c r="AC187">
+        <v>0</v>
+      </c>
+      <c r="AD187">
+        <v>0</v>
+      </c>
+      <c r="AE187">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" spans="1:31">
       <c r="A188">
@@ -19371,6 +19875,81 @@
       <c r="F188" t="s">
         <v>55</v>
       </c>
+      <c r="G188" t="s">
+        <v>353</v>
+      </c>
+      <c r="H188">
+        <v>1</v>
+      </c>
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>1</v>
+      </c>
+      <c r="K188">
+        <v>1</v>
+      </c>
+      <c r="L188">
+        <v>1</v>
+      </c>
+      <c r="M188">
+        <v>1</v>
+      </c>
+      <c r="N188">
+        <v>1</v>
+      </c>
+      <c r="O188">
+        <v>0</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="Q188">
+        <v>1</v>
+      </c>
+      <c r="R188">
+        <v>1</v>
+      </c>
+      <c r="S188">
+        <v>0</v>
+      </c>
+      <c r="T188">
+        <v>1</v>
+      </c>
+      <c r="U188">
+        <v>1</v>
+      </c>
+      <c r="V188">
+        <v>1</v>
+      </c>
+      <c r="W188">
+        <v>0</v>
+      </c>
+      <c r="X188">
+        <v>1</v>
+      </c>
+      <c r="Y188">
+        <v>1</v>
+      </c>
+      <c r="Z188">
+        <v>-1</v>
+      </c>
+      <c r="AA188">
+        <v>1</v>
+      </c>
+      <c r="AB188">
+        <v>1</v>
+      </c>
+      <c r="AC188">
+        <v>0</v>
+      </c>
+      <c r="AD188">
+        <v>0</v>
+      </c>
+      <c r="AE188">
+        <v>1</v>
+      </c>
     </row>
     <row r="189" spans="1:31">
       <c r="A189">
@@ -19391,6 +19970,81 @@
       <c r="F189" t="s">
         <v>63</v>
       </c>
+      <c r="G189" t="s">
+        <v>354</v>
+      </c>
+      <c r="H189">
+        <v>0</v>
+      </c>
+      <c r="I189">
+        <v>0</v>
+      </c>
+      <c r="J189">
+        <v>1</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
+      </c>
+      <c r="L189">
+        <v>0</v>
+      </c>
+      <c r="M189">
+        <v>0</v>
+      </c>
+      <c r="N189">
+        <v>0</v>
+      </c>
+      <c r="O189">
+        <v>0</v>
+      </c>
+      <c r="P189">
+        <v>0</v>
+      </c>
+      <c r="Q189">
+        <v>0</v>
+      </c>
+      <c r="R189">
+        <v>0</v>
+      </c>
+      <c r="S189">
+        <v>0</v>
+      </c>
+      <c r="T189">
+        <v>0</v>
+      </c>
+      <c r="U189">
+        <v>0</v>
+      </c>
+      <c r="V189">
+        <v>0</v>
+      </c>
+      <c r="W189">
+        <v>0</v>
+      </c>
+      <c r="X189">
+        <v>0</v>
+      </c>
+      <c r="Y189">
+        <v>0</v>
+      </c>
+      <c r="Z189">
+        <v>-1</v>
+      </c>
+      <c r="AA189">
+        <v>0</v>
+      </c>
+      <c r="AB189">
+        <v>0</v>
+      </c>
+      <c r="AC189">
+        <v>0</v>
+      </c>
+      <c r="AD189">
+        <v>0</v>
+      </c>
+      <c r="AE189">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" spans="1:31" s="2" customFormat="1">
       <c r="A190" s="2">
@@ -19411,6 +20065,81 @@
       <c r="F190" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="G190" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H190" s="2">
+        <v>0</v>
+      </c>
+      <c r="I190" s="2">
+        <v>0</v>
+      </c>
+      <c r="J190" s="2">
+        <v>1</v>
+      </c>
+      <c r="K190" s="2">
+        <v>0</v>
+      </c>
+      <c r="L190" s="2">
+        <v>0</v>
+      </c>
+      <c r="M190" s="2">
+        <v>0</v>
+      </c>
+      <c r="N190" s="2">
+        <v>0</v>
+      </c>
+      <c r="O190" s="2">
+        <v>0</v>
+      </c>
+      <c r="P190" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q190" s="2">
+        <v>0</v>
+      </c>
+      <c r="R190" s="2">
+        <v>0</v>
+      </c>
+      <c r="S190" s="2">
+        <v>0</v>
+      </c>
+      <c r="T190" s="2">
+        <v>0</v>
+      </c>
+      <c r="U190" s="2">
+        <v>0</v>
+      </c>
+      <c r="V190" s="2">
+        <v>0</v>
+      </c>
+      <c r="W190" s="2">
+        <v>0</v>
+      </c>
+      <c r="X190" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y190" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z190" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AA190" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB190" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC190" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD190" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE190" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" spans="1:31">
       <c r="A191">
@@ -19420,7 +20149,7 @@
         <v>23</v>
       </c>
       <c r="C191" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="D191" t="s">
         <v>85</v>
@@ -19430,6 +20159,81 @@
       </c>
       <c r="F191" t="s">
         <v>33</v>
+      </c>
+      <c r="G191" t="s">
+        <v>357</v>
+      </c>
+      <c r="H191">
+        <v>1</v>
+      </c>
+      <c r="I191">
+        <v>1</v>
+      </c>
+      <c r="J191">
+        <v>1</v>
+      </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
+      <c r="L191">
+        <v>1</v>
+      </c>
+      <c r="M191">
+        <v>0</v>
+      </c>
+      <c r="N191">
+        <v>1</v>
+      </c>
+      <c r="O191">
+        <v>0</v>
+      </c>
+      <c r="P191">
+        <v>0</v>
+      </c>
+      <c r="Q191">
+        <v>1</v>
+      </c>
+      <c r="R191">
+        <v>0</v>
+      </c>
+      <c r="S191">
+        <v>0</v>
+      </c>
+      <c r="T191">
+        <v>0</v>
+      </c>
+      <c r="U191">
+        <v>0</v>
+      </c>
+      <c r="V191">
+        <v>1</v>
+      </c>
+      <c r="W191">
+        <v>0</v>
+      </c>
+      <c r="X191">
+        <v>0</v>
+      </c>
+      <c r="Y191">
+        <v>0</v>
+      </c>
+      <c r="Z191">
+        <v>-1</v>
+      </c>
+      <c r="AA191">
+        <v>0</v>
+      </c>
+      <c r="AB191">
+        <v>0</v>
+      </c>
+      <c r="AC191">
+        <v>1</v>
+      </c>
+      <c r="AD191">
+        <v>0</v>
+      </c>
+      <c r="AE191">
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:31">
@@ -19440,7 +20244,7 @@
         <v>23</v>
       </c>
       <c r="C192" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="D192" t="s">
         <v>40</v>
@@ -19451,8 +20255,83 @@
       <c r="F192" t="s">
         <v>34</v>
       </c>
+      <c r="G192" t="s">
+        <v>359</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>1</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+      <c r="K192">
+        <v>1</v>
+      </c>
+      <c r="L192">
+        <v>1</v>
+      </c>
+      <c r="M192">
+        <v>1</v>
+      </c>
+      <c r="N192">
+        <v>1</v>
+      </c>
+      <c r="O192">
+        <v>1</v>
+      </c>
+      <c r="P192">
+        <v>1</v>
+      </c>
+      <c r="Q192">
+        <v>1</v>
+      </c>
+      <c r="R192">
+        <v>1</v>
+      </c>
+      <c r="S192">
+        <v>1</v>
+      </c>
+      <c r="T192">
+        <v>0</v>
+      </c>
+      <c r="U192">
+        <v>1</v>
+      </c>
+      <c r="V192">
+        <v>1</v>
+      </c>
+      <c r="W192">
+        <v>1</v>
+      </c>
+      <c r="X192">
+        <v>1</v>
+      </c>
+      <c r="Y192">
+        <v>1</v>
+      </c>
+      <c r="Z192">
+        <v>-1</v>
+      </c>
+      <c r="AA192">
+        <v>1</v>
+      </c>
+      <c r="AB192">
+        <v>1</v>
+      </c>
+      <c r="AC192">
+        <v>1</v>
+      </c>
+      <c r="AD192">
+        <v>1</v>
+      </c>
+      <c r="AE192">
+        <v>1</v>
+      </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:31">
       <c r="A193">
         <v>193</v>
       </c>
@@ -19460,7 +20339,7 @@
         <v>23</v>
       </c>
       <c r="C193" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="D193" t="s">
         <v>44</v>
@@ -19471,8 +20350,83 @@
       <c r="F193" t="s">
         <v>78</v>
       </c>
+      <c r="G193" t="s">
+        <v>360</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>1</v>
+      </c>
+      <c r="K193">
+        <v>1</v>
+      </c>
+      <c r="L193">
+        <v>1</v>
+      </c>
+      <c r="M193">
+        <v>1</v>
+      </c>
+      <c r="N193">
+        <v>1</v>
+      </c>
+      <c r="O193">
+        <v>1</v>
+      </c>
+      <c r="P193">
+        <v>1</v>
+      </c>
+      <c r="Q193">
+        <v>1</v>
+      </c>
+      <c r="R193">
+        <v>1</v>
+      </c>
+      <c r="S193">
+        <v>1</v>
+      </c>
+      <c r="T193">
+        <v>0</v>
+      </c>
+      <c r="U193">
+        <v>1</v>
+      </c>
+      <c r="V193">
+        <v>1</v>
+      </c>
+      <c r="W193">
+        <v>1</v>
+      </c>
+      <c r="X193">
+        <v>1</v>
+      </c>
+      <c r="Y193">
+        <v>1</v>
+      </c>
+      <c r="Z193">
+        <v>-1</v>
+      </c>
+      <c r="AA193">
+        <v>1</v>
+      </c>
+      <c r="AB193">
+        <v>1</v>
+      </c>
+      <c r="AC193">
+        <v>0</v>
+      </c>
+      <c r="AD193">
+        <v>1</v>
+      </c>
+      <c r="AE193">
+        <v>1</v>
+      </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:31">
       <c r="A194">
         <v>190</v>
       </c>
@@ -19480,7 +20434,7 @@
         <v>23</v>
       </c>
       <c r="C194" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="D194" t="s">
         <v>49</v>
@@ -19491,8 +20445,83 @@
       <c r="F194" t="s">
         <v>37</v>
       </c>
+      <c r="G194" t="s">
+        <v>362</v>
+      </c>
+      <c r="H194">
+        <v>1</v>
+      </c>
+      <c r="I194">
+        <v>0</v>
+      </c>
+      <c r="J194">
+        <v>1</v>
+      </c>
+      <c r="K194">
+        <v>0</v>
+      </c>
+      <c r="L194">
+        <v>0</v>
+      </c>
+      <c r="M194">
+        <v>0</v>
+      </c>
+      <c r="N194">
+        <v>0</v>
+      </c>
+      <c r="O194">
+        <v>1</v>
+      </c>
+      <c r="P194">
+        <v>0</v>
+      </c>
+      <c r="Q194">
+        <v>0</v>
+      </c>
+      <c r="R194">
+        <v>0</v>
+      </c>
+      <c r="S194">
+        <v>0</v>
+      </c>
+      <c r="T194">
+        <v>0</v>
+      </c>
+      <c r="U194">
+        <v>0</v>
+      </c>
+      <c r="V194">
+        <v>0</v>
+      </c>
+      <c r="W194">
+        <v>0</v>
+      </c>
+      <c r="X194">
+        <v>0</v>
+      </c>
+      <c r="Y194">
+        <v>0</v>
+      </c>
+      <c r="Z194">
+        <v>-1</v>
+      </c>
+      <c r="AA194">
+        <v>0</v>
+      </c>
+      <c r="AB194">
+        <v>0</v>
+      </c>
+      <c r="AC194">
+        <v>1</v>
+      </c>
+      <c r="AD194">
+        <v>0</v>
+      </c>
+      <c r="AE194">
+        <v>0</v>
+      </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:31">
       <c r="A195">
         <v>195</v>
       </c>
@@ -19500,7 +20529,7 @@
         <v>23</v>
       </c>
       <c r="C195" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="D195" t="s">
         <v>85</v>
@@ -19511,8 +20540,83 @@
       <c r="F195" t="s">
         <v>62</v>
       </c>
+      <c r="G195" t="s">
+        <v>364</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195">
+        <v>0</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+      <c r="K195">
+        <v>0</v>
+      </c>
+      <c r="L195">
+        <v>0</v>
+      </c>
+      <c r="M195">
+        <v>0</v>
+      </c>
+      <c r="N195">
+        <v>0</v>
+      </c>
+      <c r="O195">
+        <v>0</v>
+      </c>
+      <c r="P195">
+        <v>0</v>
+      </c>
+      <c r="Q195">
+        <v>0</v>
+      </c>
+      <c r="R195">
+        <v>0</v>
+      </c>
+      <c r="S195">
+        <v>0</v>
+      </c>
+      <c r="T195">
+        <v>0</v>
+      </c>
+      <c r="U195">
+        <v>0</v>
+      </c>
+      <c r="V195">
+        <v>0</v>
+      </c>
+      <c r="W195">
+        <v>0</v>
+      </c>
+      <c r="X195">
+        <v>0</v>
+      </c>
+      <c r="Y195">
+        <v>0</v>
+      </c>
+      <c r="Z195">
+        <v>-1</v>
+      </c>
+      <c r="AA195">
+        <v>0</v>
+      </c>
+      <c r="AB195">
+        <v>0</v>
+      </c>
+      <c r="AC195">
+        <v>0</v>
+      </c>
+      <c r="AD195">
+        <v>0</v>
+      </c>
+      <c r="AE195">
+        <v>0</v>
+      </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:31">
       <c r="A196">
         <v>197</v>
       </c>
@@ -19520,7 +20624,7 @@
         <v>23</v>
       </c>
       <c r="C196" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="D196" t="s">
         <v>72</v>
@@ -19531,8 +20635,83 @@
       <c r="F196" t="s">
         <v>66</v>
       </c>
+      <c r="G196" t="s">
+        <v>365</v>
+      </c>
+      <c r="H196">
+        <v>1</v>
+      </c>
+      <c r="I196">
+        <v>1</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+      <c r="K196">
+        <v>1</v>
+      </c>
+      <c r="L196">
+        <v>1</v>
+      </c>
+      <c r="M196">
+        <v>1</v>
+      </c>
+      <c r="N196">
+        <v>1</v>
+      </c>
+      <c r="O196">
+        <v>1</v>
+      </c>
+      <c r="P196">
+        <v>0</v>
+      </c>
+      <c r="Q196">
+        <v>1</v>
+      </c>
+      <c r="R196">
+        <v>1</v>
+      </c>
+      <c r="S196">
+        <v>1</v>
+      </c>
+      <c r="T196">
+        <v>1</v>
+      </c>
+      <c r="U196">
+        <v>0</v>
+      </c>
+      <c r="V196">
+        <v>1</v>
+      </c>
+      <c r="W196">
+        <v>1</v>
+      </c>
+      <c r="X196">
+        <v>1</v>
+      </c>
+      <c r="Y196">
+        <v>0</v>
+      </c>
+      <c r="Z196">
+        <v>-1</v>
+      </c>
+      <c r="AA196">
+        <v>1</v>
+      </c>
+      <c r="AB196">
+        <v>1</v>
+      </c>
+      <c r="AC196">
+        <v>0</v>
+      </c>
+      <c r="AD196">
+        <v>1</v>
+      </c>
+      <c r="AE196">
+        <v>1</v>
+      </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:31">
       <c r="A197">
         <v>196</v>
       </c>
@@ -19540,7 +20719,7 @@
         <v>23</v>
       </c>
       <c r="C197" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="D197" t="s">
         <v>85</v>
@@ -19551,8 +20730,83 @@
       <c r="F197" t="s">
         <v>58</v>
       </c>
+      <c r="G197" t="s">
+        <v>367</v>
+      </c>
+      <c r="H197">
+        <v>1</v>
+      </c>
+      <c r="I197">
+        <v>1</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+      <c r="K197">
+        <v>1</v>
+      </c>
+      <c r="L197">
+        <v>1</v>
+      </c>
+      <c r="M197">
+        <v>1</v>
+      </c>
+      <c r="N197">
+        <v>1</v>
+      </c>
+      <c r="O197">
+        <v>1</v>
+      </c>
+      <c r="P197">
+        <v>1</v>
+      </c>
+      <c r="Q197">
+        <v>1</v>
+      </c>
+      <c r="R197">
+        <v>1</v>
+      </c>
+      <c r="S197">
+        <v>1</v>
+      </c>
+      <c r="T197">
+        <v>1</v>
+      </c>
+      <c r="U197">
+        <v>1</v>
+      </c>
+      <c r="V197">
+        <v>1</v>
+      </c>
+      <c r="W197">
+        <v>1</v>
+      </c>
+      <c r="X197">
+        <v>1</v>
+      </c>
+      <c r="Y197">
+        <v>1</v>
+      </c>
+      <c r="Z197">
+        <v>-1</v>
+      </c>
+      <c r="AA197">
+        <v>1</v>
+      </c>
+      <c r="AB197">
+        <v>1</v>
+      </c>
+      <c r="AC197">
+        <v>1</v>
+      </c>
+      <c r="AD197">
+        <v>1</v>
+      </c>
+      <c r="AE197">
+        <v>1</v>
+      </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:31">
       <c r="A198">
         <v>194</v>
       </c>
@@ -19560,7 +20814,7 @@
         <v>23</v>
       </c>
       <c r="C198" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="D198" t="s">
         <v>49</v>
@@ -19571,8 +20825,83 @@
       <c r="F198" t="s">
         <v>42</v>
       </c>
+      <c r="G198" t="s">
+        <v>369</v>
+      </c>
+      <c r="H198">
+        <v>1</v>
+      </c>
+      <c r="I198">
+        <v>1</v>
+      </c>
+      <c r="J198">
+        <v>1</v>
+      </c>
+      <c r="K198">
+        <v>1</v>
+      </c>
+      <c r="L198">
+        <v>1</v>
+      </c>
+      <c r="M198">
+        <v>1</v>
+      </c>
+      <c r="N198">
+        <v>1</v>
+      </c>
+      <c r="O198">
+        <v>1</v>
+      </c>
+      <c r="P198">
+        <v>1</v>
+      </c>
+      <c r="Q198">
+        <v>1</v>
+      </c>
+      <c r="R198">
+        <v>1</v>
+      </c>
+      <c r="S198">
+        <v>1</v>
+      </c>
+      <c r="T198">
+        <v>1</v>
+      </c>
+      <c r="U198">
+        <v>1</v>
+      </c>
+      <c r="V198">
+        <v>1</v>
+      </c>
+      <c r="W198">
+        <v>1</v>
+      </c>
+      <c r="X198">
+        <v>1</v>
+      </c>
+      <c r="Y198">
+        <v>1</v>
+      </c>
+      <c r="Z198">
+        <v>-1</v>
+      </c>
+      <c r="AA198">
+        <v>1</v>
+      </c>
+      <c r="AB198">
+        <v>1</v>
+      </c>
+      <c r="AC198">
+        <v>1</v>
+      </c>
+      <c r="AD198">
+        <v>1</v>
+      </c>
+      <c r="AE198">
+        <v>1</v>
+      </c>
     </row>
-    <row r="199" spans="1:6" s="2" customFormat="1">
+    <row r="199" spans="1:31" s="2" customFormat="1">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -19580,7 +20909,7 @@
         <v>23</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>77</v>
@@ -19591,8 +20920,83 @@
       <c r="F199" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="G199" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H199" s="2">
+        <v>0</v>
+      </c>
+      <c r="I199" s="2">
+        <v>0</v>
+      </c>
+      <c r="J199" s="2">
+        <v>1</v>
+      </c>
+      <c r="K199" s="2">
+        <v>1</v>
+      </c>
+      <c r="L199" s="2">
+        <v>1</v>
+      </c>
+      <c r="M199" s="2">
+        <v>1</v>
+      </c>
+      <c r="N199" s="2">
+        <v>0</v>
+      </c>
+      <c r="O199" s="2">
+        <v>1</v>
+      </c>
+      <c r="P199" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q199" s="2">
+        <v>0</v>
+      </c>
+      <c r="R199" s="2">
+        <v>1</v>
+      </c>
+      <c r="S199" s="2">
+        <v>1</v>
+      </c>
+      <c r="T199" s="2">
+        <v>1</v>
+      </c>
+      <c r="U199" s="2">
+        <v>0</v>
+      </c>
+      <c r="V199" s="2">
+        <v>1</v>
+      </c>
+      <c r="W199" s="2">
+        <v>0</v>
+      </c>
+      <c r="X199" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y199" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z199" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AA199" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB199" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC199" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD199" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE199" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:31">
       <c r="A200">
         <v>199</v>
       </c>
@@ -19600,7 +21004,7 @@
         <v>24</v>
       </c>
       <c r="C200" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D200" t="s">
         <v>36</v>
@@ -19612,7 +21016,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:31">
       <c r="A201">
         <v>200</v>
       </c>
@@ -19620,7 +21024,7 @@
         <v>24</v>
       </c>
       <c r="C201" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D201" t="s">
         <v>85</v>
@@ -19632,7 +21036,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:31">
       <c r="A202">
         <v>201</v>
       </c>
@@ -19640,7 +21044,7 @@
         <v>24</v>
       </c>
       <c r="C202" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D202" t="s">
         <v>61</v>
@@ -19652,7 +21056,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:31">
       <c r="A203">
         <v>202</v>
       </c>
@@ -19660,7 +21064,7 @@
         <v>24</v>
       </c>
       <c r="C203" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D203" t="s">
         <v>185</v>
@@ -19672,7 +21076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:31">
       <c r="A204">
         <v>203</v>
       </c>
@@ -19680,7 +21084,7 @@
         <v>24</v>
       </c>
       <c r="C204" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D204" t="s">
         <v>49</v>
@@ -19692,7 +21096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:31">
       <c r="A205">
         <v>204</v>
       </c>
@@ -19700,7 +21104,7 @@
         <v>24</v>
       </c>
       <c r="C205" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D205" t="s">
         <v>49</v>
@@ -19712,7 +21116,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:31">
       <c r="A206">
         <v>205</v>
       </c>
@@ -19720,7 +21124,7 @@
         <v>24</v>
       </c>
       <c r="C206" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D206" t="s">
         <v>32</v>
@@ -19732,7 +21136,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:31">
       <c r="A207">
         <v>206</v>
       </c>
@@ -19740,7 +21144,7 @@
         <v>24</v>
       </c>
       <c r="C207" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D207" t="s">
         <v>92</v>
@@ -19752,7 +21156,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:31">
       <c r="A208">
         <v>207</v>
       </c>
@@ -19760,7 +21164,7 @@
         <v>24</v>
       </c>
       <c r="C208" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="D208" t="s">
         <v>77</v>

</xml_diff>